<commit_message>
Adding new Power BI project: Indian Retail Store Dashboard
</commit_message>
<xml_diff>
--- a/projects/excel-projects/data-visualization/e-commerce/Ecommerce_Sales_myInsights.xlsx
+++ b/projects/excel-projects/data-visualization/e-commerce/Ecommerce_Sales_myInsights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DATA_ANALYSIS\LinkedIn\e commerce\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DATA_ANALYSIS\GitHub\ZZ\Data Analytics Portfolio\projects\excel-projects\data-visualization\e-commerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1402230C-9A11-439B-A623-EB4B8A22A3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8EF8F0-20AE-401D-AFC7-C235CD72E180}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -667,16 +667,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -690,10 +689,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -885,57 +881,7 @@
           </a:sp3d>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:shade val="51000"/>
-                    <a:satMod val="130000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="80000">
-                  <a:schemeClr val="accent1">
-                    <a:shade val="93000"/>
-                    <a:satMod val="130000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:shade val="94000"/>
-                    <a:satMod val="135000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="16200000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="35000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-            <a:scene3d>
-              <a:camera prst="orthographicFront">
-                <a:rot lat="0" lon="0" rev="0"/>
-              </a:camera>
-              <a:lightRig rig="threePt" dir="t">
-                <a:rot lat="0" lon="0" rev="1200000"/>
-              </a:lightRig>
-            </a:scene3d>
-            <a:sp3d>
-              <a:bevelT w="63500" h="25400"/>
-            </a:sp3d>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -1402,22 +1348,12 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="1200">
                 <a:solidFill>
                   <a:sysClr val="window" lastClr="FFFFFF">
                     <a:lumMod val="95000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US" sz="1200"/>
@@ -1469,7 +1405,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-IN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1566,8 +1502,7 @@
           </a:sp3d>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -1603,7 +1538,7 @@
           <c:showVal val="0"/>
           <c:showCatName val="1"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
+          <c:showPercent val="1"/>
           <c:showBubbleSize val="0"/>
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
@@ -1665,19 +1600,19 @@
           <a:gradFill rotWithShape="1">
             <a:gsLst>
               <a:gs pos="0">
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:shade val="51000"/>
                   <a:satMod val="130000"/>
                 </a:schemeClr>
               </a:gs>
               <a:gs pos="80000">
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:shade val="93000"/>
                   <a:satMod val="130000"/>
                 </a:schemeClr>
               </a:gs>
               <a:gs pos="100000">
-                <a:schemeClr val="accent2">
+                <a:schemeClr val="accent1">
                   <a:shade val="94000"/>
                   <a:satMod val="135000"/>
                 </a:schemeClr>
@@ -1714,19 +1649,19 @@
           <a:gradFill rotWithShape="1">
             <a:gsLst>
               <a:gs pos="0">
-                <a:schemeClr val="accent3">
+                <a:schemeClr val="accent1">
                   <a:shade val="51000"/>
                   <a:satMod val="130000"/>
                 </a:schemeClr>
               </a:gs>
               <a:gs pos="80000">
-                <a:schemeClr val="accent3">
+                <a:schemeClr val="accent1">
                   <a:shade val="93000"/>
                   <a:satMod val="130000"/>
                 </a:schemeClr>
               </a:gs>
               <a:gs pos="100000">
-                <a:schemeClr val="accent3">
+                <a:schemeClr val="accent1">
                   <a:shade val="94000"/>
                   <a:satMod val="135000"/>
                 </a:schemeClr>
@@ -1763,19 +1698,19 @@
           <a:gradFill rotWithShape="1">
             <a:gsLst>
               <a:gs pos="0">
-                <a:schemeClr val="accent4">
+                <a:schemeClr val="accent1">
                   <a:shade val="51000"/>
                   <a:satMod val="130000"/>
                 </a:schemeClr>
               </a:gs>
               <a:gs pos="80000">
-                <a:schemeClr val="accent4">
+                <a:schemeClr val="accent1">
                   <a:shade val="93000"/>
                   <a:satMod val="130000"/>
                 </a:schemeClr>
               </a:gs>
               <a:gs pos="100000">
-                <a:schemeClr val="accent4">
+                <a:schemeClr val="accent1">
                   <a:shade val="94000"/>
                   <a:satMod val="135000"/>
                 </a:schemeClr>
@@ -2088,7 +2023,7 @@
             <c:showVal val="0"/>
             <c:showCatName val="1"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
+            <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
             <c:leaderLines>
@@ -3320,16 +3255,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3359,15 +3294,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4453,143 +4388,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{721399D1-13AE-41D5-A1D7-BF31B5D23BA5}" name="PivotTable5" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="A11:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="8">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="descending">
-      <items count="5">
-        <item x="0"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="3"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Revenue" fld="7" baseField="0" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="6">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="6" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{41975481-C918-4089-A4C1-723BFE68316F}" name="PivotTable4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{41975481-C918-4089-A4C1-723BFE68316F}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="D12:E18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -4657,7 +4456,7 @@
     <dataField name="Sum of Revenue" fld="7" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="1">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
@@ -4697,8 +4496,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{54D31A4C-121D-429B-8979-06A1964D2BA4}" name="PivotTable3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{54D31A4C-121D-429B-8979-06A1964D2BA4}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G3:H28" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -4844,8 +4643,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E3DFC5CB-3F71-4994-9B65-45A025F9DE46}" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E3DFC5CB-3F71-4994-9B65-45A025F9DE46}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D3:E9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -4924,8 +4723,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9FA9BF66-9C0E-4B90-9984-201AE1D09DEB}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9FA9BF66-9C0E-4B90-9984-201AE1D09DEB}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
   <location ref="A3:B8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -4979,6 +4778,142 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Revenue" fld="7" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <chartFormats count="6">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{721399D1-13AE-41D5-A1D7-BF31B5D23BA5}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="A11:B16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="8">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending">
+      <items count="5">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Revenue" fld="7" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="6">
     <chartFormat chart="0" format="0" series="1">
@@ -10444,7 +10379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE660FF-E2DA-49B0-846E-57A76B66356E}">
   <dimension ref="A3:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -10459,19 +10394,19 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>183</v>
       </c>
       <c r="B3" t="s">
         <v>182</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>183</v>
       </c>
       <c r="E3" t="s">
         <v>185</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>183</v>
       </c>
       <c r="H3" t="s">
@@ -10479,346 +10414,346 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>0.3756750033355189</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4">
         <v>164024.57999999996</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4">
         <v>549515.19999999995</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>0.30359593002976903</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5">
         <v>104517.54000000002</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5">
         <v>177710.36000000002</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>0.16939565073492305</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6">
         <v>92443.290000000008</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6">
         <v>155696.01999999999</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>0.15133341589978899</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7">
         <v>80324.42</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7">
         <v>120874.62</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>1</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8">
         <v>54853.42</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8">
         <v>51136.58</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9">
         <v>496163.25</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9">
         <v>44097.62</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10">
         <v>444082.19</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>183</v>
       </c>
       <c r="B11" t="s">
         <v>182</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11">
         <v>148923.16</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12">
         <v>549515.19999999995</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>183</v>
       </c>
       <c r="E12" t="s">
         <v>182</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12">
         <v>108944.64</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13">
         <v>444082.19</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>433968.44999999995</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13">
         <v>108527.8</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14">
         <v>247781.94999999998</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="7">
         <v>330272.94</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14">
         <v>54645.02</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15">
         <v>221361.57999999996</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <v>301985.86000000004</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15">
         <v>23041.57</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16">
         <v>1462740.92</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="7">
         <v>264671.53999999998</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16">
         <v>247781.95</v>
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="7">
         <v>131842.13</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17">
         <v>70139.850000000006</v>
       </c>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18">
         <v>1462740.92</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18">
         <v>68399.03</v>
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19">
         <v>46028.25</v>
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20">
         <v>41632.639999999999</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21">
         <v>21582.18</v>
       </c>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G22" s="6" t="s">
+      <c r="G22" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22">
         <v>221361.58</v>
       </c>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23">
         <v>79331.259999999995</v>
       </c>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24">
         <v>54425.43</v>
       </c>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25">
         <v>38825.229999999996</v>
       </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26">
         <v>32748.32</v>
       </c>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27">
         <v>16031.34</v>
       </c>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="G28" s="6" t="s">
+      <c r="G28" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28">
         <v>1462740.9200000002</v>
       </c>
     </row>
@@ -10831,8 +10766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69E028B8-7626-4E34-BD0B-E332991FF2B0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="X24" sqref="X24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>